<commit_message>
3_0 model success 100%
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/TRY_AGAIN_2_0/TRY_AGAIN_2_0_TEST_GAP_9/TRY_AGAIN_2_0_TEST_GAP_9_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/TRY_AGAIN_2_0/TRY_AGAIN_2_0_TEST_GAP_9/TRY_AGAIN_2_0_TEST_GAP_9_Test_Result.xlsx
@@ -445,16 +445,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.975</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>